<commit_message>
modification de la conception
</commit_message>
<xml_diff>
--- a/conception/presentation/DICTIONNAIRE.xlsx
+++ b/conception/presentation/DICTIONNAIRE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esprit/Desktop/seminaire_conception/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esprit/travail_groupe_b3/seminaire/conception/presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83687815-97C6-0C49-9CC5-1EB95EC428D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D280C-B70D-F64B-9FFF-5972A34A6986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CC5C60A9-0C08-E84C-B480-C7D6706A7625}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{CC5C60A9-0C08-E84C-B480-C7D6706A7625}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>CODE</t>
   </si>
@@ -47,102 +47,27 @@
     <t>OBSERVATION</t>
   </si>
   <si>
-    <t>ID_intervenant</t>
-  </si>
-  <si>
     <t>Prenom</t>
   </si>
   <si>
-    <t>Affectation</t>
-  </si>
-  <si>
     <t>Url</t>
   </si>
   <si>
     <t>Nom</t>
   </si>
   <si>
-    <t>Seminaire</t>
-  </si>
-  <si>
-    <t>Titre</t>
-  </si>
-  <si>
-    <t>Resume</t>
-  </si>
-  <si>
     <t>Lieu</t>
   </si>
   <si>
-    <t>Date_interrvention</t>
-  </si>
-  <si>
-    <t>Date_derniere_update</t>
-  </si>
-  <si>
-    <t>ID_calendrier</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ID_notification</t>
   </si>
   <si>
-    <t>ID_participant</t>
-  </si>
-  <si>
-    <t>Contenu</t>
-  </si>
-  <si>
     <t>ID_commentaire</t>
   </si>
   <si>
-    <t>ID_seminaire</t>
-  </si>
-  <si>
-    <t>ID de l’intervenant</t>
-  </si>
-  <si>
-    <t>Prenom intervenant</t>
-  </si>
-  <si>
     <t>Url intervenant</t>
   </si>
   <si>
-    <t>Nom intervenant</t>
-  </si>
-  <si>
-    <t>ID seminaire</t>
-  </si>
-  <si>
-    <t>Titre du seminaire</t>
-  </si>
-  <si>
-    <t>Resume de l’intervention</t>
-  </si>
-  <si>
-    <t>Lieu du seminaire</t>
-  </si>
-  <si>
-    <t>Date du l’intervention</t>
-  </si>
-  <si>
-    <t>Date derniere update</t>
-  </si>
-  <si>
-    <t>ID du calendreir</t>
-  </si>
-  <si>
-    <t>Date des evenements</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Contenu de la notification</t>
-  </si>
-  <si>
-    <t>Date du commentaire</t>
-  </si>
-  <si>
     <t>Numerique</t>
   </si>
   <si>
@@ -152,20 +77,152 @@
     <t>Aphabetique</t>
   </si>
   <si>
-    <t>id_notification_info</t>
-  </si>
-  <si>
-    <t>id_participant</t>
-  </si>
-  <si>
-    <t>id_notification</t>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>ID de l’utilisateur</t>
+  </si>
+  <si>
+    <t>Prenom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>identifient</t>
+  </si>
+  <si>
+    <t>affectation</t>
+  </si>
+  <si>
+    <t>statut de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Alphanumérique</t>
+  </si>
+  <si>
+    <t>Nom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>id_evenement</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>mdp</t>
+  </si>
+  <si>
+    <t>mot de passe utilisateur</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>telephone utilisateur</t>
+  </si>
+  <si>
+    <t>identifient de l'événément</t>
+  </si>
+  <si>
+    <t>thème</t>
+  </si>
+  <si>
+    <t>thème de l'événément</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>description de l'événément</t>
+  </si>
+  <si>
+    <t>Lieu de l'événement</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> message de la notification</t>
+  </si>
+  <si>
+    <t>date_envoie</t>
+  </si>
+  <si>
+    <t>date d'envoie de message</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>date_reception</t>
+  </si>
+  <si>
+    <t>indentifient</t>
+  </si>
+  <si>
+    <t>date_commentaire</t>
+  </si>
+  <si>
+    <t>date commentaire</t>
+  </si>
+  <si>
+    <t>contenu</t>
+  </si>
+  <si>
+    <t>contenu du commentaire</t>
+  </si>
+  <si>
+    <t>id_annonce</t>
+  </si>
+  <si>
+    <t>id annonce</t>
+  </si>
+  <si>
+    <t>numerique</t>
+  </si>
+  <si>
+    <t>date_annonce</t>
+  </si>
+  <si>
+    <t>date annonce</t>
+  </si>
+  <si>
+    <t>date_update</t>
+  </si>
+  <si>
+    <t>date mis a jours</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>tire de l'annonce</t>
+  </si>
+  <si>
+    <t>description de l'annonce</t>
+  </si>
+  <si>
+    <t>id_calendrier</t>
+  </si>
+  <si>
+    <t>id calendrier</t>
+  </si>
+  <si>
+    <t>date_clendrier</t>
+  </si>
+  <si>
+    <t>date calendrier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,21 +261,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF81D41A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFA1467E"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFFDE59"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -330,23 +372,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -358,6 +388,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,336 +707,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4112E54A-510F-3F4F-88C8-F3076ADA36DA}">
-  <dimension ref="C2:G29"/>
+  <dimension ref="C2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="3:7" s="1" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="3:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="F5" s="11">
+        <v>20</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="F6" s="11">
+        <v>20</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="F7" s="11">
+        <v>200</v>
+      </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="F8" s="11">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="F9" s="11">
+        <v>100</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="11">
+        <v>30</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="F11" s="11">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="F12" s="11">
+        <v>26</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="F14" s="11">
+        <v>27</v>
+      </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="11">
+        <v>500</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="F16" s="11">
+        <v>27</v>
+      </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="F18" s="11"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="11"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="11">
+        <v>500</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="3:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="2"/>
+      <c r="C22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="3:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C23" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="2">
+        <v>499</v>
+      </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="25" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E25" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C26" s="2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2">
+        <v>500</v>
+      </c>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="2">
+        <v>25</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="3:7" ht="19" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modification de la conception 2
</commit_message>
<xml_diff>
--- a/conception/presentation/DICTIONNAIRE.xlsx
+++ b/conception/presentation/DICTIONNAIRE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esprit/travail_groupe_b3/seminaire/conception/presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D280C-B70D-F64B-9FFF-5972A34A6986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820F5D59-BAB6-C642-B21D-BBB2B71AA926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{CC5C60A9-0C08-E84C-B480-C7D6706A7625}"/>
   </bookViews>
@@ -709,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4112E54A-510F-3F4F-88C8-F3076ADA36DA}">
   <dimension ref="C2:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>

</xml_diff>